<commit_message>
Final values for length of movement
</commit_message>
<xml_diff>
--- a/Code/Python/Video experiments/settings_deviation_from_straight.xlsx
+++ b/Code/Python/Video experiments/settings_deviation_from_straight.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Length movement" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t xml:space="preserve">avg mean</t>
   </si>
@@ -131,20 +132,19 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,4 +452,325 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>81.6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>81.78</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>80.09</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>80.18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>76.41</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>76.63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>76.65</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>77.12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>76.86</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>78.08</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>80.72</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>81.16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>79.62</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>80.09</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>79.91</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>80.26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>80.35</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>77.95</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>78.1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>79.2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>80.22</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>81.7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>73.72</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>73.72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>73.44</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>73.82</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>73.21</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>73.37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>74.04</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>74.61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>71.35</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>81.4</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>81.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>